<commit_message>
Updated Interfaces in documents.
</commit_message>
<xml_diff>
--- a/ContactsManager/Documents/SmsMmsComponent.xlsx
+++ b/ContactsManager/Documents/SmsMmsComponent.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="14355" windowHeight="4620" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="14355" windowHeight="4620" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="124">
   <si>
     <t>Deliverables</t>
   </si>
@@ -133,9 +133,6 @@
     <t>Application should be able to run or should gave graceful error and exit</t>
   </si>
   <si>
-    <t>Unit Test</t>
-  </si>
-  <si>
     <t>Run Application when there is no network connection</t>
   </si>
   <si>
@@ -163,58 +160,7 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>Get unread SMS count after the given timestamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete a SMS </t>
-  </si>
-  <si>
-    <t>Listen to SMS on port</t>
-  </si>
-  <si>
-    <t>Create SMS Broadcase Receiver, that should listen to SMS message and give callback to user module</t>
-  </si>
-  <si>
-    <t>Create Unit Test to send SMS and it should be received</t>
-  </si>
-  <si>
-    <t>Create Unit test to send SMS and it cheeck the unread SMS count</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete SMS </t>
-  </si>
-  <si>
-    <t>Delete all SMS from same caller</t>
-  </si>
-  <si>
-    <t>Create Unit Tes to send multiple SMS and delete the SMS thread</t>
-  </si>
-  <si>
-    <t>Create Unit Tes to send multiple MMS and delete the SMS thread</t>
-  </si>
-  <si>
-    <t>Create Unit test to send SMS on port and check if it is received</t>
-  </si>
-  <si>
-    <t>Send SMS</t>
-  </si>
-  <si>
-    <t>Create unit test to send sms and check if it is sent</t>
-  </si>
-  <si>
     <t>Unit Testing will be done by the developers</t>
-  </si>
-  <si>
-    <t>Get Contacts List</t>
-  </si>
-  <si>
-    <t>Get Picture associate with the contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get Contacts List </t>
-  </si>
-  <si>
-    <t>Get Picture associated with the contact</t>
   </si>
   <si>
     <t>Instead of Phone number, Contact name if present will be shown</t>
@@ -240,21 +186,6 @@
     <t>Color Code</t>
   </si>
   <si>
-    <t xml:space="preserve">Delete entire conversation from same caller </t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get complete list of conversation </t>
-  </si>
-  <si>
-    <t>Get texts of a conversation</t>
-  </si>
-  <si>
-    <t>Check SMS Service Availability</t>
-  </si>
-  <si>
     <t>User Checks for SMS connection</t>
   </si>
   <si>
@@ -336,18 +267,6 @@
     <t>Returns exception if the service initiation failed. Else starts up the service and listens for incoming sms/mms.</t>
   </si>
   <si>
-    <t>show call log for a number</t>
-  </si>
-  <si>
-    <t>delete call log for a number</t>
-  </si>
-  <si>
-    <t>all/specific</t>
-  </si>
-  <si>
-    <t>Done.Only Slight change in already built SMS receiver.</t>
-  </si>
-  <si>
     <t>com.optimus.atul.librarysms.test.LibSMSUtilsUT.libSMS</t>
   </si>
   <si>
@@ -433,6 +352,60 @@
   </si>
   <si>
     <t>com.optimus.atul.librarysms.test.LibSMSUtilsUT.tearDown()</t>
+  </si>
+  <si>
+    <t>checkSMSServiceAvailability(Context)</t>
+  </si>
+  <si>
+    <t>sendSMS(Context, String, String, Intent)</t>
+  </si>
+  <si>
+    <t>sendMMSPicture(Context, Uri, String, String)</t>
+  </si>
+  <si>
+    <t>deleteConversation(Context, String)</t>
+  </si>
+  <si>
+    <t>getListOfConversations(Context)</t>
+  </si>
+  <si>
+    <t>getTextsfromId(Context, String)</t>
+  </si>
+  <si>
+    <t>getTextsfromAddress(Context, String)</t>
+  </si>
+  <si>
+    <t>deleteSMS(Context, String)</t>
+  </si>
+  <si>
+    <t>getUnreadMessages(Context)</t>
+  </si>
+  <si>
+    <t>getContacts(Context)</t>
+  </si>
+  <si>
+    <t>getcontactEmail(Context, String)</t>
+  </si>
+  <si>
+    <t>getContactImageURI(Context, String, String)</t>
+  </si>
+  <si>
+    <t>getSMSLog(Context, String)</t>
+  </si>
+  <si>
+    <t>getCallLog(Context, String)</t>
+  </si>
+  <si>
+    <t>returns boolean</t>
+  </si>
+  <si>
+    <t>returns JSONArray</t>
+  </si>
+  <si>
+    <t>returns String</t>
+  </si>
+  <si>
+    <t>void</t>
   </si>
 </sst>
 </file>
@@ -545,7 +518,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -555,12 +528,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBFBFBF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -691,7 +658,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -808,9 +775,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -820,13 +784,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -840,7 +802,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Comma 2" xfId="5"/>
@@ -889,11 +850,11 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:axId val="80972032"/>
-        <c:axId val="80977920"/>
+        <c:axId val="43489920"/>
+        <c:axId val="43499904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80972032"/>
+        <c:axId val="43489920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -909,14 +870,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80977920"/>
+        <c:crossAx val="43499904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80977920"/>
+        <c:axId val="43499904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,14 +894,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80972032"/>
+        <c:crossAx val="43489920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -969,11 +929,11 @@
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:axId val="81272192"/>
-        <c:axId val="81294464"/>
+        <c:axId val="43802624"/>
+        <c:axId val="43804160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="81272192"/>
+        <c:axId val="43802624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -989,14 +949,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81294464"/>
+        <c:crossAx val="43804160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81294464"/>
+        <c:axId val="43804160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1013,14 +973,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="81272192"/>
+        <c:crossAx val="43802624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -1485,37 +1444,37 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="4" spans="1:7">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
     </row>
     <row r="5" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A5" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="50"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
+      <c r="A5" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="51" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
+      <c r="A8" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1564,10 +1523,10 @@
         <v>17</v>
       </c>
       <c r="C2" s="33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="33" t="s">
         <v>40</v>
-      </c>
-      <c r="D2" s="33" t="s">
-        <v>41</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>8</v>
@@ -1588,7 +1547,7 @@
         <v>18</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="38">
         <v>40</v>
@@ -1612,7 +1571,7 @@
         <v>19</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="8">
         <v>40</v>
@@ -1636,7 +1595,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="28">
         <v>40</v>
@@ -1660,7 +1619,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="28">
         <v>40</v>
@@ -1684,7 +1643,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="8">
         <v>40</v>
@@ -1708,242 +1667,205 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="47.5703125" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:4" ht="15.75">
+      <c r="A1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="44" t="s">
+      <c r="C1" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="44" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30">
-      <c r="A2" s="45">
+      <c r="D1" s="43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="44">
         <v>1</v>
       </c>
-      <c r="B2" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E2" s="46"/>
-    </row>
-    <row r="3" spans="1:5" ht="30">
-      <c r="A3" s="45">
+      <c r="B2" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="45"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="44">
         <v>2</v>
       </c>
-      <c r="B3" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="46"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="45">
+      <c r="B3" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="45"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="44">
         <v>3</v>
       </c>
-      <c r="B4" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="45" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="46"/>
-    </row>
-    <row r="5" spans="1:5" ht="30">
-      <c r="A5" s="45">
+      <c r="B4" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="45"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="44">
         <v>4</v>
       </c>
-      <c r="B5" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="46"/>
-    </row>
-    <row r="6" spans="1:5" ht="30">
-      <c r="A6" s="45">
+      <c r="B5" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="45"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="44">
         <v>5</v>
       </c>
-      <c r="B6" s="45" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="47"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="45">
+      <c r="B6" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="45"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="44">
         <v>6</v>
       </c>
-      <c r="B7" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="46"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="45">
+      <c r="B7" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="45"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="44">
         <v>7</v>
       </c>
-      <c r="B8" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E8" s="46"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="45">
+      <c r="B8" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="45"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="44">
         <v>8</v>
       </c>
-      <c r="B9" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="C9" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="46"/>
-    </row>
-    <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="45">
+      <c r="B9" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="45"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="44">
         <v>9</v>
       </c>
-      <c r="B10" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="46"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="45">
+      <c r="B10" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" s="45"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="44">
         <v>10</v>
       </c>
-      <c r="B11" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="46"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="45">
+      <c r="B11" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="45"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="44">
         <v>11</v>
       </c>
-      <c r="B12" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="46"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="45">
+      <c r="B12" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="45"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="44">
         <v>12</v>
       </c>
-      <c r="B13" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" s="46"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="45">
+      <c r="B13" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="45"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="44">
         <v>13</v>
       </c>
-      <c r="B14" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="46"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="45">
+      <c r="B14" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="45"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="44">
         <v>14</v>
       </c>
-      <c r="B15" s="45" t="s">
-        <v>101</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D15" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="46"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="45"/>
-      <c r="B16" s="45"/>
+      <c r="B15" s="44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>121</v>
+      </c>
+      <c r="D15" s="45"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1981,10 +1903,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1992,10 +1914,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="45">
@@ -2003,10 +1925,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="45">
@@ -2014,10 +1936,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>78</v>
+        <v>55</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2025,10 +1947,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60">
@@ -2036,10 +1958,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="60">
@@ -2047,10 +1969,10 @@
         <v>8</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30">
@@ -2058,10 +1980,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60">
@@ -2069,10 +1991,10 @@
         <v>10</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="C10" s="40" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="60">
@@ -2080,10 +2002,10 @@
         <v>11</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="60">
@@ -2091,10 +2013,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2102,10 +2024,10 @@
         <v>13</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2113,10 +2035,10 @@
         <v>14</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30">
@@ -2124,10 +2046,10 @@
         <v>15</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C15" s="40" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2210,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2218,7 +2140,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2226,7 +2148,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2234,7 +2156,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2242,7 +2164,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2269,15 +2191,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
+      <c r="B1" s="52"/>
       <c r="C1" s="23"/>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="53"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" ht="15.75">
       <c r="A2" s="19" t="s">
@@ -2475,7 +2397,7 @@
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="31"/>
     </row>
@@ -2485,7 +2407,7 @@
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="31"/>
     </row>
@@ -2495,7 +2417,7 @@
       </c>
       <c r="B5" s="35"/>
       <c r="C5" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5" s="31"/>
     </row>
@@ -2505,7 +2427,7 @@
       </c>
       <c r="B6" s="35"/>
       <c r="C6" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="31"/>
     </row>
@@ -2515,7 +2437,7 @@
       </c>
       <c r="B7" s="35"/>
       <c r="C7" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="31"/>
     </row>
@@ -2560,7 +2482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -2568,175 +2490,175 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>106</v>
-      </c>
-      <c r="L3" s="54"/>
+        <v>79</v>
+      </c>
+      <c r="L3" s="47"/>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>107</v>
-      </c>
-      <c r="L4" s="54"/>
+        <v>80</v>
+      </c>
+      <c r="L4" s="47"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>108</v>
-      </c>
-      <c r="L5" s="54"/>
+        <v>81</v>
+      </c>
+      <c r="L5" s="47"/>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>109</v>
-      </c>
-      <c r="L6" s="54"/>
+        <v>82</v>
+      </c>
+      <c r="L6" s="47"/>
     </row>
     <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>110</v>
-      </c>
-      <c r="L7" s="54"/>
+        <v>83</v>
+      </c>
+      <c r="L7" s="47"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>111</v>
-      </c>
-      <c r="L8" s="54"/>
+        <v>84</v>
+      </c>
+      <c r="L8" s="47"/>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>112</v>
-      </c>
-      <c r="L9" s="54"/>
+        <v>85</v>
+      </c>
+      <c r="L9" s="47"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>113</v>
-      </c>
-      <c r="L10" s="54"/>
+        <v>86</v>
+      </c>
+      <c r="L10" s="47"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>114</v>
-      </c>
-      <c r="L11" s="54"/>
+        <v>87</v>
+      </c>
+      <c r="L11" s="47"/>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>115</v>
-      </c>
-      <c r="L12" s="54"/>
+        <v>88</v>
+      </c>
+      <c r="L12" s="47"/>
     </row>
     <row r="13" spans="1:12">
       <c r="A13" t="s">
-        <v>116</v>
-      </c>
-      <c r="L13" s="54"/>
+        <v>89</v>
+      </c>
+      <c r="L13" s="47"/>
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>117</v>
-      </c>
-      <c r="L14" s="54"/>
+        <v>90</v>
+      </c>
+      <c r="L14" s="47"/>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>118</v>
-      </c>
-      <c r="L15" s="54"/>
+        <v>91</v>
+      </c>
+      <c r="L15" s="47"/>
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>119</v>
-      </c>
-      <c r="L16" s="54"/>
+        <v>92</v>
+      </c>
+      <c r="L16" s="47"/>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" t="s">
-        <v>120</v>
-      </c>
-      <c r="L17" s="54"/>
+        <v>93</v>
+      </c>
+      <c r="L17" s="47"/>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" t="s">
-        <v>121</v>
-      </c>
-      <c r="L18" s="54"/>
+        <v>94</v>
+      </c>
+      <c r="L18" s="47"/>
     </row>
     <row r="19" spans="1:12">
       <c r="A19" t="s">
-        <v>122</v>
-      </c>
-      <c r="L19" s="54"/>
+        <v>95</v>
+      </c>
+      <c r="L19" s="47"/>
     </row>
     <row r="20" spans="1:12">
       <c r="A20" t="s">
-        <v>123</v>
-      </c>
-      <c r="L20" s="54"/>
+        <v>96</v>
+      </c>
+      <c r="L20" s="47"/>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" t="s">
-        <v>124</v>
-      </c>
-      <c r="L21" s="54"/>
+        <v>97</v>
+      </c>
+      <c r="L21" s="47"/>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" t="s">
-        <v>125</v>
-      </c>
-      <c r="L22" s="54"/>
+        <v>98</v>
+      </c>
+      <c r="L22" s="47"/>
     </row>
     <row r="23" spans="1:12">
       <c r="A23" t="s">
-        <v>126</v>
-      </c>
-      <c r="L23" s="54"/>
+        <v>99</v>
+      </c>
+      <c r="L23" s="47"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" t="s">
-        <v>127</v>
-      </c>
-      <c r="L24" s="54"/>
+        <v>100</v>
+      </c>
+      <c r="L24" s="47"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
-        <v>128</v>
-      </c>
-      <c r="L25" s="54"/>
+        <v>101</v>
+      </c>
+      <c r="L25" s="47"/>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
-        <v>129</v>
-      </c>
-      <c r="L26" s="54"/>
+        <v>102</v>
+      </c>
+      <c r="L26" s="47"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" t="s">
-        <v>130</v>
-      </c>
-      <c r="L27" s="54"/>
+        <v>103</v>
+      </c>
+      <c r="L27" s="47"/>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>131</v>
-      </c>
-      <c r="L28" s="54"/>
+        <v>104</v>
+      </c>
+      <c r="L28" s="47"/>
     </row>
     <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>132</v>
-      </c>
-      <c r="L29" s="54"/>
+        <v>105</v>
+      </c>
+      <c r="L29" s="47"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>